<commit_message>
made excel export of manual validation file but may do in R
</commit_message>
<xml_diff>
--- a/metadata_files/manual_validation.xlsx
+++ b/metadata_files/manual_validation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
   <si>
     <t xml:space="preserve">cas</t>
   </si>
@@ -655,6 +655,9 @@
     <t xml:space="preserve">o-Toluidine_0_BP2.GC2_CP2551</t>
   </si>
   <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
     <t xml:space="preserve">mz0</t>
   </si>
   <si>
@@ -665,6 +668,24 @@
   </si>
   <si>
     <t xml:space="preserve">mz3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,6-Dichlorophenyl-4'-nitrophenyl ether</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-Aminobiphenyl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-aminobiphenyl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benz[a]pyrene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Di-n-octyl phthalate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azinphos ethyl</t>
   </si>
 </sst>
 </file>
@@ -5626,10 +5647,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
@@ -5638,16 +5659,16 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2">
@@ -5655,10 +5676,10 @@
         <v>100</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>102</v>
@@ -5666,12 +5687,18 @@
       <c r="E2" s="2" t="n">
         <v>10.4388</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="n">
+        <v>282.9797</v>
+      </c>
       <c r="G2" s="2" t="n">
         <v>139.0545</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="H2" s="2" t="n">
+        <v>204.015</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>254.9796</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -5681,7 +5708,7 @@
         <v>139</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>139</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>140</v>
@@ -5710,7 +5737,7 @@
         <v>139</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>149</v>
@@ -5736,10 +5763,10 @@
         <v>158</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>160</v>
@@ -5756,17 +5783,19 @@
       <c r="H5" s="2" t="n">
         <v>154.0653</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="n">
+        <v>141.0699</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
         <v>158</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>167</v>
@@ -5795,7 +5824,7 @@
         <v>177</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>177</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>178</v>
@@ -5824,7 +5853,7 @@
         <v>177</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>177</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>187</v>
@@ -5838,7 +5867,9 @@
       <c r="G8" s="2" t="n">
         <v>182.0838</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2" t="n">
+        <v>183.0872</v>
+      </c>
       <c r="I8" s="2" t="n">
         <v>181.0761</v>
       </c>
@@ -5848,10 +5879,10 @@
         <v>123</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>125</v>
@@ -5859,22 +5890,28 @@
       <c r="E9" s="2" t="n">
         <v>16.9112</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="n">
+        <v>252.0942</v>
+      </c>
       <c r="G9" s="2" t="n">
         <v>250.0786</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="H9" s="2" t="n">
+        <v>253.0974</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>248.0629</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>131</v>
@@ -5888,8 +5925,12 @@
       <c r="G10" s="2" t="n">
         <v>250.0781</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="H10" s="2" t="n">
+        <v>253.0969</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>126.0463</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
@@ -5899,7 +5940,7 @@
         <v>113</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>55</v>
+        <v>113</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>114</v>
@@ -5907,7 +5948,9 @@
       <c r="E11" s="2" t="n">
         <v>8.3914</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="n">
+        <v>433.0677</v>
+      </c>
       <c r="G11" s="2" t="n">
         <v>163.0542</v>
       </c>
@@ -5923,10 +5966,10 @@
         <v>75</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>77</v>
@@ -5940,7 +5983,9 @@
       <c r="G12" s="2" t="n">
         <v>150.1359</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2" t="n">
+        <v>275.1057</v>
+      </c>
       <c r="I12" s="2" t="n">
         <v>151.1392</v>
       </c>
@@ -5950,10 +5995,10 @@
         <v>75</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>89</v>
@@ -5961,7 +6006,9 @@
       <c r="E13" s="2" t="n">
         <v>14.1913</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="n">
+        <v>149.0238</v>
+      </c>
       <c r="G13" s="2" t="n">
         <v>279.159</v>
       </c>
@@ -5977,10 +6024,10 @@
         <v>105</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>107</v>
@@ -5994,116 +6041,68 @@
       <c r="G14" s="2" t="n">
         <v>104.0495</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="H14" s="2" t="n">
+        <v>137.0056</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>133.0477</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>123</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>125</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>16.9112</v>
+        <v>5.797</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>252.0942</v>
+        <v>106.0653</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>250.0786</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+        <v>107.073</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>108.0683</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>105.0573</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>123</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>16.6163</v>
+        <v>7.8706</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>252.0937</v>
+        <v>107.073</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>250.0781</v>
-      </c>
-      <c r="H16" s="2"/>
+        <v>106.0651</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>108.0764</v>
+      </c>
       <c r="I16" s="2" t="n">
-        <v>126.0463</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>5.797</v>
-      </c>
-      <c r="F17" s="2" t="n">
-        <v>106.0653</v>
-      </c>
-      <c r="G17" s="2" t="n">
-        <v>107.073</v>
-      </c>
-      <c r="H17" s="2" t="n">
-        <v>108.0683</v>
-      </c>
-      <c r="I17" s="2" t="n">
-        <v>105.0573</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>7.8706</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>107.073</v>
-      </c>
-      <c r="G18" s="2" t="n">
-        <v>106.0651</v>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>108.0764</v>
-      </c>
-      <c r="I18" s="2" t="n">
         <v>105.0336</v>
       </c>
     </row>

</xml_diff>